<commit_message>
Fixed Pert and Gantt diagrams for Project-plan and Team-plan
</commit_message>
<xml_diff>
--- a/1ο Παραδοτέο/Project-Plan/Files/Project-plan.xlsx
+++ b/1ο Παραδοτέο/Project-Plan/Files/Project-plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Greg\University-Software-Engineering-Project\1ο Παραδοτέο\Project-Plan\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3849910-94E9-4ED6-BF82-E06823A605EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CF7C35-0414-45C1-B7C6-7C671A39D450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1EAC7372-4E6D-4560-AE19-81BB16F488F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
   <si>
     <t>TY 1</t>
   </si>
@@ -233,18 +233,6 @@
     <t>Wed 13/03/24</t>
   </si>
   <si>
-    <t>Wed 24/04/24</t>
-  </si>
-  <si>
-    <t>Tue 21/05/24</t>
-  </si>
-  <si>
-    <t>Wed 22/05/24</t>
-  </si>
-  <si>
-    <t>Tue 13/08/24</t>
-  </si>
-  <si>
     <t>Mon 20/03/23</t>
   </si>
   <si>
@@ -290,37 +278,22 @@
     <t>Tue 12/03/24</t>
   </si>
   <si>
-    <t>Tue 23/04/24</t>
-  </si>
-  <si>
-    <t>Tue 06/08/24</t>
-  </si>
-  <si>
-    <t>Ορόσημο 1: Τέλος Αρχικής Ανάλυσης</t>
-  </si>
-  <si>
-    <t>Ορόσημο 2: Τέλος Αρχικού Σχεδιασμού</t>
-  </si>
-  <si>
-    <t>Ορόσημο 3: Τέλος Αρχικής Ανάπτυξης Εφαρμογής</t>
-  </si>
-  <si>
-    <t>Ορόσημο 4: Τέλος φάσης προετοιμασίας για κοινοποίηση - Κοινοποίηση Εφαρμογής</t>
-  </si>
-  <si>
     <t>TY 6</t>
   </si>
   <si>
-    <t>TY 22</t>
-  </si>
-  <si>
-    <t>TY 23</t>
-  </si>
-  <si>
-    <t>TY 24</t>
-  </si>
-  <si>
-    <t>TY 25</t>
+    <t>Tue 27/02/24</t>
+  </si>
+  <si>
+    <t>Wed 10/04/24</t>
+  </si>
+  <si>
+    <t>Tue 09/04/24</t>
+  </si>
+  <si>
+    <t>Tue 02/07/24</t>
+  </si>
+  <si>
+    <t>Tue 25/06/24</t>
   </si>
 </sst>
 </file>
@@ -399,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -409,9 +382,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,7 +700,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,7 +756,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1">
         <v>14</v>
@@ -818,7 +788,7 @@
         <v>51</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1">
         <v>7</v>
@@ -830,11 +800,11 @@
         <v>10</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3:H6" si="0">((G3-F3)/6)^2</f>
+        <f t="shared" ref="H3:H5" si="0">((G3-F3)/6)^2</f>
         <v>1.3611111111111114</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I6" si="1">(F3+4*E3+G3)/6</f>
+        <f t="shared" ref="I3:I5" si="1">(F3+4*E3+G3)/6</f>
         <v>6.833333333333333</v>
       </c>
       <c r="J3" s="1"/>
@@ -844,30 +814,30 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="E4" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
       </c>
       <c r="G4" s="1">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="0"/>
-        <v>1.3611111111111114</v>
+        <f>((G4-F4)/6)^2</f>
+        <v>4</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="1"/>
-        <v>6.833333333333333</v>
+        <f>(F4+4*E4+G4)/6</f>
+        <v>9.6666666666666661</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -876,30 +846,30 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="E5" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1">
         <v>3</v>
       </c>
       <c r="G5" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1.3611111111111114</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>9.6666666666666661</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="J5" s="1"/>
     </row>
@@ -908,62 +878,62 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="H6:H12" si="2">((G6-F6)/6)^2</f>
+        <v>2.7777777777777781</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="I6:I12" si="3">(F6+4*E6+G6)/6</f>
+        <v>13.333333333333334</v>
       </c>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H7" s="1">
-        <f>((G7-F7)/6)^2</f>
-        <v>2.7777777777777781</v>
+        <f t="shared" si="2"/>
+        <v>2.25</v>
       </c>
       <c r="I7" s="1">
-        <f>(F7+4*E7+G7)/6</f>
-        <v>13.333333333333334</v>
+        <f t="shared" si="3"/>
+        <v>9.5</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -972,7 +942,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>54</v>
@@ -981,21 +951,21 @@
         <v>73</v>
       </c>
       <c r="E8" s="1">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G8" s="1">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="H8" s="1">
         <f>((G8-F8)/6)^2</f>
-        <v>2.25</v>
+        <v>38.027777777777779</v>
       </c>
       <c r="I8" s="1">
         <f>(F8+4*E8+G8)/6</f>
-        <v>9.5</v>
+        <v>31.166666666666668</v>
       </c>
       <c r="J8" s="1"/>
     </row>
@@ -1010,7 +980,7 @@
         <v>55</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E9" s="1">
         <v>14</v>
@@ -1022,11 +992,11 @@
         <v>18</v>
       </c>
       <c r="H9" s="1">
-        <f>((G9-F9)/6)^2</f>
+        <f t="shared" si="2"/>
         <v>3.3611111111111107</v>
       </c>
       <c r="I9" s="1">
-        <f>(F9+4*E9+G9)/6</f>
+        <f t="shared" si="3"/>
         <v>13.5</v>
       </c>
       <c r="J9" s="1"/>
@@ -1042,7 +1012,7 @@
         <v>56</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E10" s="1">
         <v>14</v>
@@ -1054,11 +1024,11 @@
         <v>17</v>
       </c>
       <c r="H10" s="1">
-        <f>((G10-F10)/6)^2</f>
+        <f t="shared" si="2"/>
         <v>2.7777777777777781</v>
       </c>
       <c r="I10" s="1">
-        <f>(F10+4*E10+G10)/6</f>
+        <f t="shared" si="3"/>
         <v>13.333333333333334</v>
       </c>
       <c r="J10" s="1"/>
@@ -1086,11 +1056,11 @@
         <v>13</v>
       </c>
       <c r="H11" s="1">
-        <f>((G11-F11)/6)^2</f>
+        <f t="shared" si="2"/>
         <v>2.25</v>
       </c>
       <c r="I11" s="1">
-        <f>(F11+4*E11+G11)/6</f>
+        <f t="shared" si="3"/>
         <v>9.5</v>
       </c>
       <c r="J11" s="1"/>
@@ -1106,7 +1076,7 @@
         <v>57</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E12" s="1">
         <v>7</v>
@@ -1118,11 +1088,11 @@
         <v>10</v>
       </c>
       <c r="H12" s="1">
-        <f>((G12-F12)/6)^2</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I12" s="1">
-        <f>(F12+4*E12+G12)/6</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="J12" s="1"/>
@@ -1132,30 +1102,30 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E13" s="1">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G13" s="1">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="H13" s="1">
         <f>((G13-F13)/6)^2</f>
-        <v>38.027777777777779</v>
+        <v>34.027777777777771</v>
       </c>
       <c r="I13" s="1">
         <f>(F13+4*E13+G13)/6</f>
-        <v>31.166666666666668</v>
+        <v>39.166666666666664</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -1164,30 +1134,30 @@
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H14" s="1">
         <f>((G14-F14)/6)^2</f>
-        <v>0</v>
+        <v>26.694444444444446</v>
       </c>
       <c r="I14" s="1">
         <f>(F14+4*E14+G14)/6</f>
-        <v>0</v>
+        <v>33.166666666666664</v>
       </c>
       <c r="J14" s="1"/>
     </row>
@@ -1196,30 +1166,30 @@
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E15" s="1">
+        <v>30</v>
+      </c>
+      <c r="F15" s="1">
+        <v>7</v>
+      </c>
+      <c r="G15" s="1">
         <v>40</v>
-      </c>
-      <c r="F15" s="1">
-        <v>20</v>
-      </c>
-      <c r="G15" s="1">
-        <v>55</v>
       </c>
       <c r="H15" s="1">
         <f>((G15-F15)/6)^2</f>
-        <v>34.027777777777771</v>
+        <v>30.25</v>
       </c>
       <c r="I15" s="1">
         <f>(F15+4*E15+G15)/6</f>
-        <v>39.166666666666664</v>
+        <v>27.833333333333332</v>
       </c>
       <c r="J15" s="1"/>
     </row>
@@ -1228,30 +1198,30 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E16" s="1">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F16" s="1">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="G16" s="1">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="H16" s="1">
         <f>((G16-F16)/6)^2</f>
-        <v>26.694444444444446</v>
+        <v>25</v>
       </c>
       <c r="I16" s="1">
         <f>(F16+4*E16+G16)/6</f>
-        <v>33.166666666666664</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="J16" s="1"/>
     </row>
@@ -1260,30 +1230,30 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="1">
+        <v>40</v>
+      </c>
+      <c r="F17" s="1">
+        <v>30</v>
+      </c>
+      <c r="G17" s="1">
         <v>60</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="1">
-        <v>30</v>
-      </c>
-      <c r="F17" s="1">
-        <v>7</v>
-      </c>
-      <c r="G17" s="1">
-        <v>40</v>
       </c>
       <c r="H17" s="1">
         <f>((G17-F17)/6)^2</f>
-        <v>30.25</v>
+        <v>25</v>
       </c>
       <c r="I17" s="1">
         <f>(F17+4*E17+G17)/6</f>
-        <v>27.833333333333332</v>
+        <v>41.666666666666664</v>
       </c>
       <c r="J17" s="1"/>
     </row>
@@ -1292,13 +1262,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E18" s="1">
         <v>40</v>
@@ -1324,30 +1294,30 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E19" s="1">
+        <v>30</v>
+      </c>
+      <c r="F19" s="1">
+        <v>15</v>
+      </c>
+      <c r="G19" s="1">
         <v>40</v>
-      </c>
-      <c r="F19" s="1">
-        <v>30</v>
-      </c>
-      <c r="G19" s="1">
-        <v>60</v>
       </c>
       <c r="H19" s="1">
         <f>((G19-F19)/6)^2</f>
-        <v>25</v>
+        <v>17.361111111111114</v>
       </c>
       <c r="I19" s="1">
         <f>(F19+4*E19+G19)/6</f>
-        <v>41.666666666666664</v>
+        <v>29.166666666666668</v>
       </c>
       <c r="J19" s="1"/>
     </row>
@@ -1356,30 +1326,30 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>83</v>
       </c>
       <c r="E20" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F20" s="1">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="G20" s="1">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="H20" s="1">
         <f>((G20-F20)/6)^2</f>
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="I20" s="1">
         <f>(F20+4*E20+G20)/6</f>
-        <v>41.666666666666664</v>
+        <v>18.666666666666668</v>
       </c>
       <c r="J20" s="1"/>
     </row>
@@ -1388,30 +1358,30 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E21" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F21" s="1">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="G21" s="1">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="H21" s="1">
         <f>((G21-F21)/6)^2</f>
-        <v>17.361111111111114</v>
+        <v>56.25</v>
       </c>
       <c r="I21" s="1">
         <f>(F21+4*E21+G21)/6</f>
-        <v>29.166666666666668</v>
+        <v>62.5</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -1420,157 +1390,46 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="1">
+        <v>55</v>
+      </c>
+      <c r="F22" s="1">
         <v>45</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="1">
-        <v>20</v>
-      </c>
-      <c r="F22" s="1">
-        <v>7</v>
-      </c>
       <c r="G22" s="1">
-        <v>25</v>
+        <v>80</v>
       </c>
       <c r="H22" s="1">
         <f>((G22-F22)/6)^2</f>
-        <v>9</v>
+        <v>34.027777777777771</v>
       </c>
       <c r="I22" s="1">
         <f>(F22+4*E22+G22)/6</f>
-        <v>18.666666666666668</v>
+        <v>57.5</v>
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <f>((G23-F23)/6)^2</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="1">
-        <f>(F23+4*E23+G23)/6</f>
-        <v>0</v>
-      </c>
-    </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="1">
-        <v>60</v>
-      </c>
-      <c r="F24" s="1">
-        <v>45</v>
-      </c>
-      <c r="G24" s="1">
-        <v>90</v>
-      </c>
-      <c r="H24" s="1">
-        <f>((G24-F24)/6)^2</f>
-        <v>56.25</v>
-      </c>
-      <c r="I24" s="1">
-        <f>(F24+4*E24+G24)/6</f>
-        <v>62.5</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="1">
-        <v>55</v>
-      </c>
-      <c r="F25" s="1">
-        <v>45</v>
-      </c>
-      <c r="G25" s="1">
-        <v>80</v>
-      </c>
-      <c r="H25" s="1">
-        <f>((G25-F25)/6)^2</f>
-        <v>34.027777777777771</v>
-      </c>
-      <c r="I25" s="1">
-        <f>(F25+4*E25+G25)/6</f>
-        <v>57.5</v>
-      </c>
       <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-      <c r="F26" s="1">
-        <v>0</v>
-      </c>
-      <c r="G26" s="1">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1">
-        <f>((G26-F26)/6)^2</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="4">
-        <f>(F26+4*E26+G26)/6</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>

</xml_diff>